<commit_message>
mises a jour info
</commit_message>
<xml_diff>
--- a/ToM/compVsMimic_Etude/EtudeFinale/dataToRemove.xlsx
+++ b/ToM/compVsMimic_Etude/EtudeFinale/dataToRemove.xlsx
@@ -168,7 +168,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -270,12 +270,18 @@
       <c r="I3" s="0" t="n">
         <v>7</v>
       </c>
+      <c r="J3" s="0" t="n">
+        <v>7</v>
+      </c>
       <c r="L3" s="0" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H4" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="J4" s="0" t="n">
         <v>28</v>
       </c>
       <c r="L4" s="0" t="n">

</xml_diff>